<commit_message>
update: generator + static lib
Update initialization function
Update app_types_data.xlsx for bit masks
Update static lib files (.c, .h, .a)
</commit_message>
<xml_diff>
--- a/generator/app_types_data.xlsx
+++ b/generator/app_types_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
   <si>
     <t>TYPES</t>
   </si>
@@ -77,8 +77,8 @@
   </si>
   <si>
     <t>CHASSIS_ISSUE_NONE = 0,
-CHASSIS_ISSUE_TYRES = 1,
-CHASSIS_ISSUE_BRAKES = 2</t>
+CHASSIS_ISSUE_TYRES = (1 &lt;&lt; 0),
+CHASSIS_ISSUE_BRAKES = (1 &lt;&lt; 1)</t>
   </si>
   <si>
     <t>Chassis issues</t>
@@ -107,9 +107,9 @@
   </si>
   <si>
     <t>MOTOR_ISSUE_NONE = 0,
-MOTOR_ISSUE_TYRES = 1,
-MOTOR_ISSUE_TEMPERATURE_LDR = 2,
-MOTOR_ISSUE_OIL_OVERHEATING = 4</t>
+MOTOR_ISSUE_TYRES = (1 &lt;&lt; 0),
+MOTOR_ISSUE_TEMPERATURE_LDR = (1 &lt;&lt; 1),
+MOTOR_ISSUE_OIL_OVERHEATING = (1 &lt;&lt; 2)</t>
   </si>
   <si>
     <t>Motor issues</t>
@@ -161,9 +161,9 @@
     <t>battery_issues_t</t>
   </si>
   <si>
-    <t>BATTERY_ISSUES_NONE = 0x0,
-BATTERY_ISSUES_DISCHARGED = 0x1,
-BATTERY_ISSUES_KO = 0x2</t>
+    <t>BATTERY_ISSUES_NONE = 0,
+BATTERY_ISSUES_DISCHARGED = (1 &lt;&lt; 0),
+BATTERY_ISSUES_KO = (1 &lt;&lt; 1)</t>
   </si>
   <si>
     <t>Battery issues</t>
@@ -197,26 +197,40 @@
     <t>bcgv_bgf_msg_id_t</t>
   </si>
   <si>
-    <t>BCGV_BGF_MSG_ID_1 = 0x01,
-BCGV_BGF_MSG_ID_2 = 0x02,
-BCGV_BGF_MSG_ID_3 = 0x03,
-BCGV_BGF_MSG_ID_4 = 0x04,
-BCGV_BGF_MSG_ID_5 = 0x05</t>
+    <t>BCGV_BGF_MSG_ID_1 = 1,
+BCGV_BGF_MSG_ID_2 = 2,
+BCGV_BGF_MSG_ID_3 = 3,
+BCGV_BGF_MSG_ID_4 = 4,
+BCGV_BGF_MSG_ID_5 = 5</t>
   </si>
   <si>
     <t>[BCGV -&gt; BGF] Message ID</t>
   </si>
   <si>
+    <t>flag_t</t>
+  </si>
+  <si>
+    <t>[BCGV -&gt; MUX] Alert flag</t>
+  </si>
+  <si>
     <t>bit_flag_t</t>
   </si>
   <si>
     <t xml:space="preserve">Bit-carrying flag </t>
   </si>
   <si>
-    <t>flag_t</t>
-  </si>
-  <si>
-    <t>[BCGV -&gt; MUX] Alert flag</t>
+    <t>bgf_ack_t</t>
+  </si>
+  <si>
+    <t>BGF_ACK_POSITION_LIGHT = (1 &lt;&lt; 0),
+BGF_ACK_CROSSING_LIGHT = (1 &lt;&lt; 1),
+BGF_ACK_HIGHBEAM_LIGHT = (1 &lt;&lt; 2),
+BGF_ACK_INDIC_LEFT = (1 &lt;&lt; 3),
+BGF_ACK_INDIC_RIGHT = (1 &lt;&lt; 4),
+BGF_ACK_INDIC_HAZARD = (1 &lt;&lt; 5)</t>
+  </si>
+  <si>
+    <t>BGF message acknowledgement bits</t>
   </si>
   <si>
     <t>DONNEES</t>
@@ -369,7 +383,7 @@
     <t>bit_flag_bgf_ack</t>
   </si>
   <si>
-    <t>BGF flags set as bits, bit-carrying</t>
+    <t>BGF acknowledgement flags, bit-carrying</t>
   </si>
 </sst>
 </file>
@@ -431,7 +445,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border/>
     <border>
       <left style="medium">
@@ -784,13 +798,24 @@
       </top>
       <bottom style="thick">
         <color rgb="FFFF0000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF434343"/>
       </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -968,6 +993,9 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="32" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1194,7 +1222,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="3.25"/>
     <col customWidth="1" min="2" max="3" width="19.75"/>
-    <col customWidth="1" min="4" max="4" width="36.25"/>
+    <col customWidth="1" min="4" max="4" width="40.63"/>
     <col customWidth="1" min="5" max="5" width="18.38"/>
     <col customWidth="1" min="6" max="6" width="75.0"/>
     <col customWidth="1" min="7" max="7" width="47.75"/>
@@ -1517,7 +1545,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E16" s="44"/>
       <c r="F16" s="45" t="s">
@@ -1554,7 +1582,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E17" s="44"/>
       <c r="F17" s="45" t="s">
@@ -1582,64 +1610,82 @@
       <c r="Z17" s="46"/>
       <c r="AA17" s="46"/>
     </row>
-    <row r="20">
-      <c r="A20" s="1"/>
-      <c r="B20" s="47" t="s">
+    <row r="18">
+      <c r="A18" s="41"/>
+      <c r="B18" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="5"/>
+      <c r="C18" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="44"/>
+      <c r="F18" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="46"/>
+      <c r="S18" s="46"/>
+      <c r="T18" s="46"/>
+      <c r="U18" s="46"/>
+      <c r="V18" s="46"/>
+      <c r="W18" s="46"/>
+      <c r="X18" s="46"/>
+      <c r="Y18" s="46"/>
+      <c r="Z18" s="46"/>
+      <c r="AA18" s="46"/>
     </row>
     <row r="21">
-      <c r="A21" s="2"/>
-      <c r="B21" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="49" t="s">
+      <c r="A21" s="1"/>
+      <c r="B21" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2"/>
+      <c r="B22" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="50" t="s">
+      <c r="D22" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="50" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="51"/>
-      <c r="B22" s="52">
-        <v>1.0</v>
-      </c>
-      <c r="C22" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53">
-        <v>0.0</v>
-      </c>
-      <c r="G22" s="55" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="51"/>
       <c r="B23" s="52">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C23" s="53" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D23" s="54" t="s">
         <v>6</v>
@@ -1649,16 +1695,16 @@
         <v>0.0</v>
       </c>
       <c r="G23" s="55" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="51"/>
-      <c r="B24" s="56">
-        <v>3.0</v>
+      <c r="B24" s="52">
+        <v>2.0</v>
       </c>
       <c r="C24" s="53" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D24" s="54" t="s">
         <v>6</v>
@@ -1668,16 +1714,16 @@
         <v>0.0</v>
       </c>
       <c r="G24" s="55" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="51"/>
       <c r="B25" s="56">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C25" s="53" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D25" s="54" t="s">
         <v>6</v>
@@ -1687,16 +1733,16 @@
         <v>0.0</v>
       </c>
       <c r="G25" s="55" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="51"/>
-      <c r="B26" s="52">
-        <v>5.0</v>
+      <c r="B26" s="56">
+        <v>4.0</v>
       </c>
       <c r="C26" s="53" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D26" s="54" t="s">
         <v>6</v>
@@ -1706,54 +1752,54 @@
         <v>0.0</v>
       </c>
       <c r="G26" s="55" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="51"/>
       <c r="B27" s="52">
-        <v>6.0</v>
-      </c>
-      <c r="C27" s="54" t="s">
-        <v>64</v>
+        <v>5.0</v>
+      </c>
+      <c r="C27" s="53" t="s">
+        <v>65</v>
       </c>
       <c r="D27" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54">
+      <c r="E27" s="53"/>
+      <c r="F27" s="53">
         <v>0.0</v>
       </c>
-      <c r="G27" s="57" t="s">
-        <v>65</v>
+      <c r="G27" s="55" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="51"/>
       <c r="B28" s="52">
-        <v>7.0</v>
-      </c>
-      <c r="C28" s="53" t="s">
-        <v>66</v>
+        <v>6.0</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>67</v>
       </c>
       <c r="D28" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53">
+      <c r="E28" s="54"/>
+      <c r="F28" s="54">
         <v>0.0</v>
       </c>
-      <c r="G28" s="55" t="s">
-        <v>67</v>
+      <c r="G28" s="57" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="51"/>
-      <c r="B29" s="56">
-        <v>8.0</v>
+      <c r="B29" s="52">
+        <v>7.0</v>
       </c>
       <c r="C29" s="53" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D29" s="54" t="s">
         <v>6</v>
@@ -1763,92 +1809,92 @@
         <v>0.0</v>
       </c>
       <c r="G29" s="55" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="51"/>
-      <c r="B30" s="52">
-        <v>9.0</v>
+      <c r="B30" s="56">
+        <v>8.0</v>
       </c>
       <c r="C30" s="53" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D30" s="54" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E30" s="53"/>
       <c r="F30" s="53">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G30" s="55" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="51"/>
       <c r="B31" s="52">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="C31" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58">
-        <v>0.0</v>
+        <v>73</v>
+      </c>
+      <c r="D31" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53">
+        <v>1.0</v>
       </c>
       <c r="G31" s="55" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="51"/>
-      <c r="B32" s="56">
-        <v>11.0</v>
+      <c r="B32" s="52">
+        <v>10.0</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D32" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53">
+        <v>14</v>
+      </c>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58">
         <v>0.0</v>
       </c>
       <c r="G32" s="55" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="51"/>
-      <c r="B33" s="52">
-        <v>12.0</v>
+      <c r="B33" s="56">
+        <v>11.0</v>
       </c>
       <c r="C33" s="53" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D33" s="53" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E33" s="53"/>
       <c r="F33" s="53">
         <v>0.0</v>
       </c>
       <c r="G33" s="55" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="51"/>
       <c r="B34" s="52">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="C34" s="53" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D34" s="53" t="s">
         <v>28</v>
@@ -1858,215 +1904,234 @@
         <v>0.0</v>
       </c>
       <c r="G34" s="55" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="51"/>
-      <c r="B35" s="56">
-        <v>14.0</v>
+      <c r="B35" s="52">
+        <v>13.0</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D35" s="53" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E35" s="53"/>
       <c r="F35" s="53">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="G35" s="55" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="51"/>
-      <c r="B36" s="52">
-        <v>15.0</v>
-      </c>
-      <c r="C36" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="59" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59">
-        <v>0.0</v>
-      </c>
-      <c r="G36" s="60" t="s">
+      <c r="B36" s="56">
+        <v>14.0</v>
+      </c>
+      <c r="C36" s="53" t="s">
         <v>81</v>
+      </c>
+      <c r="D36" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53">
+        <v>40.0</v>
+      </c>
+      <c r="G36" s="55" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="51"/>
       <c r="B37" s="52">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="C37" s="59" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D37" s="59" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E37" s="59"/>
       <c r="F37" s="59">
         <v>0.0</v>
       </c>
       <c r="G37" s="60" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="51"/>
-      <c r="B38" s="56">
-        <v>17.0</v>
+      <c r="B38" s="52">
+        <v>16.0</v>
       </c>
       <c r="C38" s="59" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D38" s="59" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E38" s="59"/>
       <c r="F38" s="59">
         <v>0.0</v>
       </c>
       <c r="G38" s="60" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="52">
-        <v>18.0</v>
+      <c r="A39" s="51"/>
+      <c r="B39" s="56">
+        <v>17.0</v>
       </c>
       <c r="C39" s="59" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D39" s="59" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E39" s="59"/>
       <c r="F39" s="59">
         <v>0.0</v>
       </c>
       <c r="G39" s="60" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40">
-      <c r="B40" s="56">
-        <v>19.0</v>
+      <c r="B40" s="52">
+        <v>18.0</v>
       </c>
       <c r="C40" s="59" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D40" s="59" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E40" s="59"/>
       <c r="F40" s="59">
         <v>0.0</v>
       </c>
       <c r="G40" s="60" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41">
-      <c r="B41" s="52">
-        <v>20.0</v>
+      <c r="B41" s="56">
+        <v>19.0</v>
       </c>
       <c r="C41" s="59" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D41" s="59" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E41" s="59"/>
       <c r="F41" s="59">
         <v>0.0</v>
       </c>
       <c r="G41" s="60" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="56">
-        <v>21.0</v>
+      <c r="B42" s="52">
+        <v>20.0</v>
       </c>
       <c r="C42" s="59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D42" s="59" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E42" s="59"/>
       <c r="F42" s="59">
         <v>0.0</v>
       </c>
       <c r="G42" s="60" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43">
-      <c r="B43" s="52">
-        <v>22.0</v>
+      <c r="B43" s="56">
+        <v>21.0</v>
       </c>
       <c r="C43" s="59" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D43" s="59" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E43" s="59"/>
       <c r="F43" s="59">
         <v>0.0</v>
       </c>
       <c r="G43" s="60" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44">
-      <c r="B44" s="56">
-        <v>23.0</v>
+      <c r="B44" s="52">
+        <v>22.0</v>
       </c>
       <c r="C44" s="59" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D44" s="59" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E44" s="59"/>
       <c r="F44" s="59">
         <v>0.0</v>
       </c>
       <c r="G44" s="60" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="56">
+        <v>23.0</v>
+      </c>
+      <c r="C45" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59">
+        <v>0.0</v>
+      </c>
+      <c r="G45" s="60" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" s="61">
         <v>24.0</v>
       </c>
-      <c r="C45" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61">
+      <c r="C46" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" s="62"/>
+      <c r="F46" s="62">
         <v>0.0</v>
       </c>
-      <c r="G45" s="62" t="s">
-        <v>99</v>
+      <c r="G46" s="63" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>